<commit_message>
Almost added all the tables (still formatting remains)
</commit_message>
<xml_diff>
--- a/wyniki/merged_in_order.xlsx
+++ b/wyniki/merged_in_order.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\uczelnia\magister\PRACA DYPLOMOWA\wyniki\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25354664-AECF-43EE-98CF-12DE17BA4687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D196BF9-DDA4-4F27-9534-823AE240DC9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{8D03BF68-5000-4F71-B9A7-7FF09177C41F}"/>
   </bookViews>
@@ -20,158 +20,158 @@
     <sheet name="formB descriptive" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'formA descriptive'!$AA$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'formA descriptive'!$AA$2:$AA$15</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">'formA descriptive'!$AF$1</definedName>
-    <definedName name="_xlchart.v1.100" hidden="1">'formB descriptive'!$M$1</definedName>
-    <definedName name="_xlchart.v1.101" hidden="1">'formB descriptive'!$M$2:$M$21</definedName>
-    <definedName name="_xlchart.v1.102" hidden="1">'formB descriptive'!$N$1</definedName>
-    <definedName name="_xlchart.v1.103" hidden="1">'formB descriptive'!$N$2:$N$21</definedName>
-    <definedName name="_xlchart.v1.104" hidden="1">'formB descriptive'!$O$1</definedName>
-    <definedName name="_xlchart.v1.105" hidden="1">'formB descriptive'!$O$2:$O$21</definedName>
-    <definedName name="_xlchart.v1.106" hidden="1">'formB descriptive'!$P$1</definedName>
-    <definedName name="_xlchart.v1.107" hidden="1">'formB descriptive'!$P$2:$P$21</definedName>
-    <definedName name="_xlchart.v1.108" hidden="1">'formB descriptive'!$Q$1</definedName>
-    <definedName name="_xlchart.v1.109" hidden="1">'formB descriptive'!$Q$2:$Q$21</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">'formA descriptive'!$AF$2:$AF$15</definedName>
-    <definedName name="_xlchart.v1.110" hidden="1">'formB descriptive'!$R$1</definedName>
-    <definedName name="_xlchart.v1.111" hidden="1">'formB descriptive'!$R$2:$R$21</definedName>
-    <definedName name="_xlchart.v1.112" hidden="1">'formB descriptive'!$S$1</definedName>
-    <definedName name="_xlchart.v1.113" hidden="1">'formB descriptive'!$S$2:$S$21</definedName>
-    <definedName name="_xlchart.v1.114" hidden="1">'formB descriptive'!$AA$1</definedName>
-    <definedName name="_xlchart.v1.115" hidden="1">'formB descriptive'!$AA$2:$AA$21</definedName>
-    <definedName name="_xlchart.v1.116" hidden="1">'formB descriptive'!$AB$1</definedName>
-    <definedName name="_xlchart.v1.117" hidden="1">'formB descriptive'!$AB$2:$AB$21</definedName>
-    <definedName name="_xlchart.v1.118" hidden="1">'formB descriptive'!$AC$1</definedName>
-    <definedName name="_xlchart.v1.119" hidden="1">'formB descriptive'!$AC$2:$AC$21</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">'formA descriptive'!$AG$1</definedName>
-    <definedName name="_xlchart.v1.120" hidden="1">'formB descriptive'!$AD$1</definedName>
-    <definedName name="_xlchart.v1.121" hidden="1">'formB descriptive'!$AD$2:$AD$21</definedName>
-    <definedName name="_xlchart.v1.122" hidden="1">'formB descriptive'!$AE$1</definedName>
-    <definedName name="_xlchart.v1.123" hidden="1">'formB descriptive'!$AE$2:$AE$21</definedName>
-    <definedName name="_xlchart.v1.124" hidden="1">'formB descriptive'!$AF$1</definedName>
-    <definedName name="_xlchart.v1.125" hidden="1">'formB descriptive'!$AF$2:$AF$21</definedName>
-    <definedName name="_xlchart.v1.126" hidden="1">'formB descriptive'!$AG$1</definedName>
-    <definedName name="_xlchart.v1.127" hidden="1">'formB descriptive'!$AG$2:$AG$21</definedName>
-    <definedName name="_xlchart.v1.128" hidden="1">'formB descriptive'!$AH$1</definedName>
-    <definedName name="_xlchart.v1.129" hidden="1">'formB descriptive'!$AH$2:$AH$21</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">'formA descriptive'!$AG$2:$AG$15</definedName>
-    <definedName name="_xlchart.v1.130" hidden="1">'formB descriptive'!$AI$1</definedName>
-    <definedName name="_xlchart.v1.131" hidden="1">'formB descriptive'!$AI$2:$AI$21</definedName>
-    <definedName name="_xlchart.v1.132" hidden="1">'formB descriptive'!$AJ$1</definedName>
-    <definedName name="_xlchart.v1.133" hidden="1">'formB descriptive'!$AJ$2:$AJ$21</definedName>
-    <definedName name="_xlchart.v1.134" hidden="1">'formB descriptive'!$AK$1</definedName>
-    <definedName name="_xlchart.v1.135" hidden="1">'formB descriptive'!$AK$2:$AK$21</definedName>
-    <definedName name="_xlchart.v1.136" hidden="1">'formB descriptive'!$AL$1</definedName>
-    <definedName name="_xlchart.v1.137" hidden="1">'formB descriptive'!$AL$2:$AL$21</definedName>
-    <definedName name="_xlchart.v1.138" hidden="1">'formB descriptive'!$AM$1</definedName>
-    <definedName name="_xlchart.v1.139" hidden="1">'formB descriptive'!$AM$2:$AM$21</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">'formA descriptive'!$AH$1</definedName>
-    <definedName name="_xlchart.v1.140" hidden="1">'formB descriptive'!$U$1</definedName>
-    <definedName name="_xlchart.v1.141" hidden="1">'formB descriptive'!$U$2:$U$21</definedName>
-    <definedName name="_xlchart.v1.142" hidden="1">'formB descriptive'!$V$1</definedName>
-    <definedName name="_xlchart.v1.143" hidden="1">'formB descriptive'!$V$2:$V$21</definedName>
-    <definedName name="_xlchart.v1.144" hidden="1">'formB descriptive'!$W$1</definedName>
-    <definedName name="_xlchart.v1.145" hidden="1">'formB descriptive'!$W$2:$W$21</definedName>
-    <definedName name="_xlchart.v1.146" hidden="1">'formB descriptive'!$X$1</definedName>
-    <definedName name="_xlchart.v1.147" hidden="1">'formB descriptive'!$X$2:$X$21</definedName>
-    <definedName name="_xlchart.v1.148" hidden="1">'formB descriptive'!$Y$1</definedName>
-    <definedName name="_xlchart.v1.149" hidden="1">'formB descriptive'!$Y$2:$Y$21</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">'formA descriptive'!$AH$2:$AH$15</definedName>
-    <definedName name="_xlchart.v1.150" hidden="1">'formB descriptive'!$Z$1</definedName>
-    <definedName name="_xlchart.v1.151" hidden="1">'formB descriptive'!$Z$2:$Z$21</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">'formA descriptive'!$AI$1</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">'formA descriptive'!$AI$2:$AI$15</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">'formA descriptive'!$AJ$1</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">'formA descriptive'!$AJ$2:$AJ$15</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'formA descriptive'!$AB$1</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">'formA descriptive'!$AK$1</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">'formA descriptive'!$AK$2:$AK$15</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">'formA descriptive'!$AL$1</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">'formA descriptive'!$AL$2:$AL$15</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">'formA descriptive'!$AM$1</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">'formA descriptive'!$AM$2:$AM$15</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">'formA descriptive'!$U$1</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">'formA descriptive'!$U$2:$U$15</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">'formA descriptive'!$V$1</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">'formA descriptive'!$V$2:$V$15</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'formA descriptive'!$AB$2:$AB$15</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">'formA descriptive'!$W$1</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">'formA descriptive'!$W$2:$W$15</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">'formA descriptive'!$X$1</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">'formA descriptive'!$X$2:$X$15</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">'formA descriptive'!$Y$1</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">'formA descriptive'!$Y$2:$Y$15</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">'formA descriptive'!$Z$1</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">'formA descriptive'!$Z$2:$Z$15</definedName>
-    <definedName name="_xlchart.v1.38" hidden="1">'formA descriptive'!$A$1</definedName>
-    <definedName name="_xlchart.v1.39" hidden="1">'formA descriptive'!$A$2:$A$15</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'formA descriptive'!$AC$1</definedName>
-    <definedName name="_xlchart.v1.40" hidden="1">'formA descriptive'!$B$1</definedName>
-    <definedName name="_xlchart.v1.41" hidden="1">'formA descriptive'!$B$2:$B$15</definedName>
-    <definedName name="_xlchart.v1.42" hidden="1">'formA descriptive'!$C$1</definedName>
-    <definedName name="_xlchart.v1.43" hidden="1">'formA descriptive'!$C$2:$C$15</definedName>
-    <definedName name="_xlchart.v1.44" hidden="1">'formA descriptive'!$D$1</definedName>
-    <definedName name="_xlchart.v1.45" hidden="1">'formA descriptive'!$D$2:$D$15</definedName>
-    <definedName name="_xlchart.v1.46" hidden="1">'formA descriptive'!$E$1</definedName>
-    <definedName name="_xlchart.v1.47" hidden="1">'formA descriptive'!$E$2:$E$15</definedName>
-    <definedName name="_xlchart.v1.48" hidden="1">'formA descriptive'!$F$1</definedName>
-    <definedName name="_xlchart.v1.49" hidden="1">'formA descriptive'!$F$2:$F$15</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'formA descriptive'!$AC$2:$AC$15</definedName>
-    <definedName name="_xlchart.v1.50" hidden="1">'formA descriptive'!$G$1</definedName>
-    <definedName name="_xlchart.v1.51" hidden="1">'formA descriptive'!$G$2:$G$15</definedName>
-    <definedName name="_xlchart.v1.52" hidden="1">'formA descriptive'!$H$1</definedName>
-    <definedName name="_xlchart.v1.53" hidden="1">'formA descriptive'!$H$2:$H$15</definedName>
-    <definedName name="_xlchart.v1.54" hidden="1">'formA descriptive'!$I$1</definedName>
-    <definedName name="_xlchart.v1.55" hidden="1">'formA descriptive'!$I$2:$I$15</definedName>
-    <definedName name="_xlchart.v1.56" hidden="1">'formA descriptive'!$J$1</definedName>
-    <definedName name="_xlchart.v1.57" hidden="1">'formA descriptive'!$J$2:$J$15</definedName>
-    <definedName name="_xlchart.v1.58" hidden="1">'formA descriptive'!$K$1</definedName>
-    <definedName name="_xlchart.v1.59" hidden="1">'formA descriptive'!$K$2:$K$15</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'formA descriptive'!$AD$1</definedName>
-    <definedName name="_xlchart.v1.60" hidden="1">'formA descriptive'!$L$1</definedName>
-    <definedName name="_xlchart.v1.61" hidden="1">'formA descriptive'!$L$2:$L$15</definedName>
-    <definedName name="_xlchart.v1.62" hidden="1">'formA descriptive'!$M$1</definedName>
-    <definedName name="_xlchart.v1.63" hidden="1">'formA descriptive'!$M$2:$M$15</definedName>
-    <definedName name="_xlchart.v1.64" hidden="1">'formA descriptive'!$N$1</definedName>
-    <definedName name="_xlchart.v1.65" hidden="1">'formA descriptive'!$N$2:$N$15</definedName>
-    <definedName name="_xlchart.v1.66" hidden="1">'formA descriptive'!$O$1</definedName>
-    <definedName name="_xlchart.v1.67" hidden="1">'formA descriptive'!$O$2:$O$15</definedName>
-    <definedName name="_xlchart.v1.68" hidden="1">'formA descriptive'!$P$1</definedName>
-    <definedName name="_xlchart.v1.69" hidden="1">'formA descriptive'!$P$2:$P$15</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'formA descriptive'!$AD$2:$AD$15</definedName>
-    <definedName name="_xlchart.v1.70" hidden="1">'formA descriptive'!$Q$1</definedName>
-    <definedName name="_xlchart.v1.71" hidden="1">'formA descriptive'!$Q$2:$Q$15</definedName>
-    <definedName name="_xlchart.v1.72" hidden="1">'formA descriptive'!$R$1</definedName>
-    <definedName name="_xlchart.v1.73" hidden="1">'formA descriptive'!$R$2:$R$15</definedName>
-    <definedName name="_xlchart.v1.74" hidden="1">'formA descriptive'!$S$1</definedName>
-    <definedName name="_xlchart.v1.75" hidden="1">'formA descriptive'!$S$2:$S$15</definedName>
-    <definedName name="_xlchart.v1.76" hidden="1">'formB descriptive'!$A$1</definedName>
-    <definedName name="_xlchart.v1.77" hidden="1">'formB descriptive'!$A$2:$A$21</definedName>
-    <definedName name="_xlchart.v1.78" hidden="1">'formB descriptive'!$B$1</definedName>
-    <definedName name="_xlchart.v1.79" hidden="1">'formB descriptive'!$B$2:$B$21</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'formA descriptive'!$AE$1</definedName>
-    <definedName name="_xlchart.v1.80" hidden="1">'formB descriptive'!$C$1</definedName>
-    <definedName name="_xlchart.v1.81" hidden="1">'formB descriptive'!$C$2:$C$21</definedName>
-    <definedName name="_xlchart.v1.82" hidden="1">'formB descriptive'!$D$1</definedName>
-    <definedName name="_xlchart.v1.83" hidden="1">'formB descriptive'!$D$2:$D$21</definedName>
-    <definedName name="_xlchart.v1.84" hidden="1">'formB descriptive'!$E$1</definedName>
-    <definedName name="_xlchart.v1.85" hidden="1">'formB descriptive'!$E$2:$E$21</definedName>
-    <definedName name="_xlchart.v1.86" hidden="1">'formB descriptive'!$F$1</definedName>
-    <definedName name="_xlchart.v1.87" hidden="1">'formB descriptive'!$F$2:$F$21</definedName>
-    <definedName name="_xlchart.v1.88" hidden="1">'formB descriptive'!$G$1</definedName>
-    <definedName name="_xlchart.v1.89" hidden="1">'formB descriptive'!$G$2:$G$21</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'formA descriptive'!$AE$2:$AE$15</definedName>
-    <definedName name="_xlchart.v1.90" hidden="1">'formB descriptive'!$H$1</definedName>
-    <definedName name="_xlchart.v1.91" hidden="1">'formB descriptive'!$H$2:$H$21</definedName>
-    <definedName name="_xlchart.v1.92" hidden="1">'formB descriptive'!$I$1</definedName>
-    <definedName name="_xlchart.v1.93" hidden="1">'formB descriptive'!$I$2:$I$21</definedName>
-    <definedName name="_xlchart.v1.94" hidden="1">'formB descriptive'!$J$1</definedName>
-    <definedName name="_xlchart.v1.95" hidden="1">'formB descriptive'!$J$2:$J$21</definedName>
-    <definedName name="_xlchart.v1.96" hidden="1">'formB descriptive'!$K$1</definedName>
-    <definedName name="_xlchart.v1.97" hidden="1">'formB descriptive'!$K$2:$K$21</definedName>
-    <definedName name="_xlchart.v1.98" hidden="1">'formB descriptive'!$L$1</definedName>
-    <definedName name="_xlchart.v1.99" hidden="1">'formB descriptive'!$L$2:$L$21</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">'formA descriptive'!$A$1</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'formA descriptive'!$A$2:$A$15</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">'formA descriptive'!$F$1</definedName>
+    <definedName name="_xlchart.v1.100" hidden="1">'formB descriptive'!$AM$1</definedName>
+    <definedName name="_xlchart.v1.101" hidden="1">'formB descriptive'!$AM$2:$AM$21</definedName>
+    <definedName name="_xlchart.v1.102" hidden="1">'formB descriptive'!$U$1</definedName>
+    <definedName name="_xlchart.v1.103" hidden="1">'formB descriptive'!$U$2:$U$21</definedName>
+    <definedName name="_xlchart.v1.104" hidden="1">'formB descriptive'!$V$1</definedName>
+    <definedName name="_xlchart.v1.105" hidden="1">'formB descriptive'!$V$2:$V$21</definedName>
+    <definedName name="_xlchart.v1.106" hidden="1">'formB descriptive'!$W$1</definedName>
+    <definedName name="_xlchart.v1.107" hidden="1">'formB descriptive'!$W$2:$W$21</definedName>
+    <definedName name="_xlchart.v1.108" hidden="1">'formB descriptive'!$X$1</definedName>
+    <definedName name="_xlchart.v1.109" hidden="1">'formB descriptive'!$X$2:$X$21</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">'formA descriptive'!$F$2:$F$15</definedName>
+    <definedName name="_xlchart.v1.110" hidden="1">'formB descriptive'!$Y$1</definedName>
+    <definedName name="_xlchart.v1.111" hidden="1">'formB descriptive'!$Y$2:$Y$21</definedName>
+    <definedName name="_xlchart.v1.112" hidden="1">'formB descriptive'!$Z$1</definedName>
+    <definedName name="_xlchart.v1.113" hidden="1">'formB descriptive'!$Z$2:$Z$21</definedName>
+    <definedName name="_xlchart.v1.114" hidden="1">'formB descriptive'!$A$1</definedName>
+    <definedName name="_xlchart.v1.115" hidden="1">'formB descriptive'!$A$2:$A$21</definedName>
+    <definedName name="_xlchart.v1.116" hidden="1">'formB descriptive'!$B$1</definedName>
+    <definedName name="_xlchart.v1.117" hidden="1">'formB descriptive'!$B$2:$B$21</definedName>
+    <definedName name="_xlchart.v1.118" hidden="1">'formB descriptive'!$C$1</definedName>
+    <definedName name="_xlchart.v1.119" hidden="1">'formB descriptive'!$C$2:$C$21</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">'formA descriptive'!$G$1</definedName>
+    <definedName name="_xlchart.v1.120" hidden="1">'formB descriptive'!$D$1</definedName>
+    <definedName name="_xlchart.v1.121" hidden="1">'formB descriptive'!$D$2:$D$21</definedName>
+    <definedName name="_xlchart.v1.122" hidden="1">'formB descriptive'!$E$1</definedName>
+    <definedName name="_xlchart.v1.123" hidden="1">'formB descriptive'!$E$2:$E$21</definedName>
+    <definedName name="_xlchart.v1.124" hidden="1">'formB descriptive'!$F$1</definedName>
+    <definedName name="_xlchart.v1.125" hidden="1">'formB descriptive'!$F$2:$F$21</definedName>
+    <definedName name="_xlchart.v1.126" hidden="1">'formB descriptive'!$G$1</definedName>
+    <definedName name="_xlchart.v1.127" hidden="1">'formB descriptive'!$G$2:$G$21</definedName>
+    <definedName name="_xlchart.v1.128" hidden="1">'formB descriptive'!$H$1</definedName>
+    <definedName name="_xlchart.v1.129" hidden="1">'formB descriptive'!$H$2:$H$21</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">'formA descriptive'!$G$2:$G$15</definedName>
+    <definedName name="_xlchart.v1.130" hidden="1">'formB descriptive'!$I$1</definedName>
+    <definedName name="_xlchart.v1.131" hidden="1">'formB descriptive'!$I$2:$I$21</definedName>
+    <definedName name="_xlchart.v1.132" hidden="1">'formB descriptive'!$J$1</definedName>
+    <definedName name="_xlchart.v1.133" hidden="1">'formB descriptive'!$J$2:$J$21</definedName>
+    <definedName name="_xlchart.v1.134" hidden="1">'formB descriptive'!$K$1</definedName>
+    <definedName name="_xlchart.v1.135" hidden="1">'formB descriptive'!$K$2:$K$21</definedName>
+    <definedName name="_xlchart.v1.136" hidden="1">'formB descriptive'!$L$1</definedName>
+    <definedName name="_xlchart.v1.137" hidden="1">'formB descriptive'!$L$2:$L$21</definedName>
+    <definedName name="_xlchart.v1.138" hidden="1">'formB descriptive'!$M$1</definedName>
+    <definedName name="_xlchart.v1.139" hidden="1">'formB descriptive'!$M$2:$M$21</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">'formA descriptive'!$H$1</definedName>
+    <definedName name="_xlchart.v1.140" hidden="1">'formB descriptive'!$N$1</definedName>
+    <definedName name="_xlchart.v1.141" hidden="1">'formB descriptive'!$N$2:$N$21</definedName>
+    <definedName name="_xlchart.v1.142" hidden="1">'formB descriptive'!$O$1</definedName>
+    <definedName name="_xlchart.v1.143" hidden="1">'formB descriptive'!$O$2:$O$21</definedName>
+    <definedName name="_xlchart.v1.144" hidden="1">'formB descriptive'!$P$1</definedName>
+    <definedName name="_xlchart.v1.145" hidden="1">'formB descriptive'!$P$2:$P$21</definedName>
+    <definedName name="_xlchart.v1.146" hidden="1">'formB descriptive'!$Q$1</definedName>
+    <definedName name="_xlchart.v1.147" hidden="1">'formB descriptive'!$Q$2:$Q$21</definedName>
+    <definedName name="_xlchart.v1.148" hidden="1">'formB descriptive'!$R$1</definedName>
+    <definedName name="_xlchart.v1.149" hidden="1">'formB descriptive'!$R$2:$R$21</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">'formA descriptive'!$H$2:$H$15</definedName>
+    <definedName name="_xlchart.v1.150" hidden="1">'formB descriptive'!$S$1</definedName>
+    <definedName name="_xlchart.v1.151" hidden="1">'formB descriptive'!$S$2:$S$21</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">'formA descriptive'!$I$1</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">'formA descriptive'!$I$2:$I$15</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">'formA descriptive'!$J$1</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">'formA descriptive'!$J$2:$J$15</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'formA descriptive'!$B$1</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">'formA descriptive'!$K$1</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">'formA descriptive'!$K$2:$K$15</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">'formA descriptive'!$L$1</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">'formA descriptive'!$L$2:$L$15</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">'formA descriptive'!$M$1</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">'formA descriptive'!$M$2:$M$15</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">'formA descriptive'!$N$1</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">'formA descriptive'!$N$2:$N$15</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">'formA descriptive'!$O$1</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">'formA descriptive'!$O$2:$O$15</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'formA descriptive'!$B$2:$B$15</definedName>
+    <definedName name="_xlchart.v1.30" hidden="1">'formA descriptive'!$P$1</definedName>
+    <definedName name="_xlchart.v1.31" hidden="1">'formA descriptive'!$P$2:$P$15</definedName>
+    <definedName name="_xlchart.v1.32" hidden="1">'formA descriptive'!$Q$1</definedName>
+    <definedName name="_xlchart.v1.33" hidden="1">'formA descriptive'!$Q$2:$Q$15</definedName>
+    <definedName name="_xlchart.v1.34" hidden="1">'formA descriptive'!$R$1</definedName>
+    <definedName name="_xlchart.v1.35" hidden="1">'formA descriptive'!$R$2:$R$15</definedName>
+    <definedName name="_xlchart.v1.36" hidden="1">'formA descriptive'!$S$1</definedName>
+    <definedName name="_xlchart.v1.37" hidden="1">'formA descriptive'!$S$2:$S$15</definedName>
+    <definedName name="_xlchart.v1.38" hidden="1">'formA descriptive'!$AA$1</definedName>
+    <definedName name="_xlchart.v1.39" hidden="1">'formA descriptive'!$AA$2:$AA$15</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'formA descriptive'!$C$1</definedName>
+    <definedName name="_xlchart.v1.40" hidden="1">'formA descriptive'!$AB$1</definedName>
+    <definedName name="_xlchart.v1.41" hidden="1">'formA descriptive'!$AB$2:$AB$15</definedName>
+    <definedName name="_xlchart.v1.42" hidden="1">'formA descriptive'!$AC$1</definedName>
+    <definedName name="_xlchart.v1.43" hidden="1">'formA descriptive'!$AC$2:$AC$15</definedName>
+    <definedName name="_xlchart.v1.44" hidden="1">'formA descriptive'!$AD$1</definedName>
+    <definedName name="_xlchart.v1.45" hidden="1">'formA descriptive'!$AD$2:$AD$15</definedName>
+    <definedName name="_xlchart.v1.46" hidden="1">'formA descriptive'!$AE$1</definedName>
+    <definedName name="_xlchart.v1.47" hidden="1">'formA descriptive'!$AE$2:$AE$15</definedName>
+    <definedName name="_xlchart.v1.48" hidden="1">'formA descriptive'!$AF$1</definedName>
+    <definedName name="_xlchart.v1.49" hidden="1">'formA descriptive'!$AF$2:$AF$15</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'formA descriptive'!$C$2:$C$15</definedName>
+    <definedName name="_xlchart.v1.50" hidden="1">'formA descriptive'!$AG$1</definedName>
+    <definedName name="_xlchart.v1.51" hidden="1">'formA descriptive'!$AG$2:$AG$15</definedName>
+    <definedName name="_xlchart.v1.52" hidden="1">'formA descriptive'!$AH$1</definedName>
+    <definedName name="_xlchart.v1.53" hidden="1">'formA descriptive'!$AH$2:$AH$15</definedName>
+    <definedName name="_xlchart.v1.54" hidden="1">'formA descriptive'!$AI$1</definedName>
+    <definedName name="_xlchart.v1.55" hidden="1">'formA descriptive'!$AI$2:$AI$15</definedName>
+    <definedName name="_xlchart.v1.56" hidden="1">'formA descriptive'!$AJ$1</definedName>
+    <definedName name="_xlchart.v1.57" hidden="1">'formA descriptive'!$AJ$2:$AJ$15</definedName>
+    <definedName name="_xlchart.v1.58" hidden="1">'formA descriptive'!$AK$1</definedName>
+    <definedName name="_xlchart.v1.59" hidden="1">'formA descriptive'!$AK$2:$AK$15</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'formA descriptive'!$D$1</definedName>
+    <definedName name="_xlchart.v1.60" hidden="1">'formA descriptive'!$AL$1</definedName>
+    <definedName name="_xlchart.v1.61" hidden="1">'formA descriptive'!$AL$2:$AL$15</definedName>
+    <definedName name="_xlchart.v1.62" hidden="1">'formA descriptive'!$AM$1</definedName>
+    <definedName name="_xlchart.v1.63" hidden="1">'formA descriptive'!$AM$2:$AM$15</definedName>
+    <definedName name="_xlchart.v1.64" hidden="1">'formA descriptive'!$U$1</definedName>
+    <definedName name="_xlchart.v1.65" hidden="1">'formA descriptive'!$U$2:$U$15</definedName>
+    <definedName name="_xlchart.v1.66" hidden="1">'formA descriptive'!$V$1</definedName>
+    <definedName name="_xlchart.v1.67" hidden="1">'formA descriptive'!$V$2:$V$15</definedName>
+    <definedName name="_xlchart.v1.68" hidden="1">'formA descriptive'!$W$1</definedName>
+    <definedName name="_xlchart.v1.69" hidden="1">'formA descriptive'!$W$2:$W$15</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'formA descriptive'!$D$2:$D$15</definedName>
+    <definedName name="_xlchart.v1.70" hidden="1">'formA descriptive'!$X$1</definedName>
+    <definedName name="_xlchart.v1.71" hidden="1">'formA descriptive'!$X$2:$X$15</definedName>
+    <definedName name="_xlchart.v1.72" hidden="1">'formA descriptive'!$Y$1</definedName>
+    <definedName name="_xlchart.v1.73" hidden="1">'formA descriptive'!$Y$2:$Y$15</definedName>
+    <definedName name="_xlchart.v1.74" hidden="1">'formA descriptive'!$Z$1</definedName>
+    <definedName name="_xlchart.v1.75" hidden="1">'formA descriptive'!$Z$2:$Z$15</definedName>
+    <definedName name="_xlchart.v1.76" hidden="1">'formB descriptive'!$AA$1</definedName>
+    <definedName name="_xlchart.v1.77" hidden="1">'formB descriptive'!$AA$2:$AA$21</definedName>
+    <definedName name="_xlchart.v1.78" hidden="1">'formB descriptive'!$AB$1</definedName>
+    <definedName name="_xlchart.v1.79" hidden="1">'formB descriptive'!$AB$2:$AB$21</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">'formA descriptive'!$E$1</definedName>
+    <definedName name="_xlchart.v1.80" hidden="1">'formB descriptive'!$AC$1</definedName>
+    <definedName name="_xlchart.v1.81" hidden="1">'formB descriptive'!$AC$2:$AC$21</definedName>
+    <definedName name="_xlchart.v1.82" hidden="1">'formB descriptive'!$AD$1</definedName>
+    <definedName name="_xlchart.v1.83" hidden="1">'formB descriptive'!$AD$2:$AD$21</definedName>
+    <definedName name="_xlchart.v1.84" hidden="1">'formB descriptive'!$AE$1</definedName>
+    <definedName name="_xlchart.v1.85" hidden="1">'formB descriptive'!$AE$2:$AE$21</definedName>
+    <definedName name="_xlchart.v1.86" hidden="1">'formB descriptive'!$AF$1</definedName>
+    <definedName name="_xlchart.v1.87" hidden="1">'formB descriptive'!$AF$2:$AF$21</definedName>
+    <definedName name="_xlchart.v1.88" hidden="1">'formB descriptive'!$AG$1</definedName>
+    <definedName name="_xlchart.v1.89" hidden="1">'formB descriptive'!$AG$2:$AG$21</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">'formA descriptive'!$E$2:$E$15</definedName>
+    <definedName name="_xlchart.v1.90" hidden="1">'formB descriptive'!$AH$1</definedName>
+    <definedName name="_xlchart.v1.91" hidden="1">'formB descriptive'!$AH$2:$AH$21</definedName>
+    <definedName name="_xlchart.v1.92" hidden="1">'formB descriptive'!$AI$1</definedName>
+    <definedName name="_xlchart.v1.93" hidden="1">'formB descriptive'!$AI$2:$AI$21</definedName>
+    <definedName name="_xlchart.v1.94" hidden="1">'formB descriptive'!$AJ$1</definedName>
+    <definedName name="_xlchart.v1.95" hidden="1">'formB descriptive'!$AJ$2:$AJ$21</definedName>
+    <definedName name="_xlchart.v1.96" hidden="1">'formB descriptive'!$AK$1</definedName>
+    <definedName name="_xlchart.v1.97" hidden="1">'formB descriptive'!$AK$2:$AK$21</definedName>
+    <definedName name="_xlchart.v1.98" hidden="1">'formB descriptive'!$AL$1</definedName>
+    <definedName name="_xlchart.v1.99" hidden="1">'formB descriptive'!$AL$2:$AL$21</definedName>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">combined!$A$1:$BC$35</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -4094,97 +4094,97 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.39</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.41</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.43</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.45</cx:f>
+        <cx:f>_xlchart.v1.7</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="4">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.47</cx:f>
+        <cx:f>_xlchart.v1.9</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="5">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.49</cx:f>
+        <cx:f>_xlchart.v1.11</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="6">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.51</cx:f>
+        <cx:f>_xlchart.v1.13</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="7">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.53</cx:f>
+        <cx:f>_xlchart.v1.15</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="8">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.55</cx:f>
+        <cx:f>_xlchart.v1.17</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="9">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.57</cx:f>
+        <cx:f>_xlchart.v1.19</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="10">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.59</cx:f>
+        <cx:f>_xlchart.v1.21</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="11">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.61</cx:f>
+        <cx:f>_xlchart.v1.23</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="12">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.63</cx:f>
+        <cx:f>_xlchart.v1.25</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="13">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.65</cx:f>
+        <cx:f>_xlchart.v1.27</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="14">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.67</cx:f>
+        <cx:f>_xlchart.v1.29</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="15">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.69</cx:f>
+        <cx:f>_xlchart.v1.31</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="16">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.71</cx:f>
+        <cx:f>_xlchart.v1.33</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="17">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.73</cx:f>
+        <cx:f>_xlchart.v1.35</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="18">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.75</cx:f>
+        <cx:f>_xlchart.v1.37</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -4194,7 +4194,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{14DB9EF3-7C72-49A1-86F8-744E79F81050}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.38</cx:f>
+              <cx:f>_xlchart.v1.0</cx:f>
               <cx:v>I lose track of time</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4218,7 +4218,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{28954439-E554-499B-A931-7DD5E4FE2398}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.40</cx:f>
+              <cx:f>_xlchart.v1.2</cx:f>
               <cx:v>I was interested in the game's story</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4241,7 +4241,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{5FDB13A7-697C-45B5-BBD7-1BF9362EF47D}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.42</cx:f>
+              <cx:f>_xlchart.v1.4</cx:f>
               <cx:v>I feel different </cx:v>
             </cx:txData>
           </cx:tx>
@@ -4263,7 +4263,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{D8D1F8AA-37EE-4BCD-BD16-3EECE70FB4F6}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.44</cx:f>
+              <cx:f>_xlchart.v1.6</cx:f>
               <cx:v>I felt that I could explore things</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4285,7 +4285,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{76DD44DE-EB10-48DE-9D62-3E8CBCBCA526}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.46</cx:f>
+              <cx:f>_xlchart.v1.8</cx:f>
               <cx:v>The game feels real</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4307,7 +4307,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{BB15A01C-5E33-4E8D-BD27-6DC1C6ECBE8B}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.48</cx:f>
+              <cx:f>_xlchart.v1.10</cx:f>
               <cx:v>I was fully occupied with the game</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4329,7 +4329,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{FE1EF1A2-DE25-4837-B56F-0723CAC5CD08}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.50</cx:f>
+              <cx:f>_xlchart.v1.12</cx:f>
               <cx:v>I get wound up</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4351,7 +4351,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{80A22390-F0DE-4AA5-921B-A88BD8AD65DF}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.52</cx:f>
+              <cx:f>_xlchart.v1.14</cx:f>
               <cx:v>Time seems to kind of stand still or stop</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4382,7 +4382,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{7C541C84-D642-49DE-9497-26343A07203C}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.54</cx:f>
+              <cx:f>_xlchart.v1.16</cx:f>
               <cx:v>I feel spaced out</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4404,7 +4404,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{FB399FAA-0903-4292-B99E-C97B26E3AE17}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.56</cx:f>
+              <cx:f>_xlchart.v1.18</cx:f>
               <cx:v>I was deeply concentrated in the game</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4426,7 +4426,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{3564EB1B-CD8C-4860-8938-6C3449A4F1D2}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.58</cx:f>
+              <cx:f>_xlchart.v1.20</cx:f>
               <cx:v>I got tired</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4448,7 +4448,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{15B77A2A-3E29-48ED-9669-4B55CF92978A}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.60</cx:f>
+              <cx:f>_xlchart.v1.22</cx:f>
               <cx:v>Playing seems automatic</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4470,7 +4470,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{6D05807E-D4DC-4997-ACB8-1A2979E78A51}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.62</cx:f>
+              <cx:f>_xlchart.v1.24</cx:f>
               <cx:v>My thoughts go fast</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4492,7 +4492,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{CC6CD2DE-F2C0-491E-A106-795600B33B76}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.64</cx:f>
+              <cx:f>_xlchart.v1.26</cx:f>
               <cx:v>I enjoyed it</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4514,7 +4514,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{308F09CE-DC95-4014-91CC-6C3AAA923D76}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.66</cx:f>
+              <cx:f>_xlchart.v1.28</cx:f>
               <cx:v>I play without thinking how to play</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4536,7 +4536,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{CA9904C7-CF78-484C-9758-BEC54BCA8F14}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.68</cx:f>
+              <cx:f>_xlchart.v1.30</cx:f>
               <cx:v>Playing makes me feel calm</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4558,7 +4558,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{63C92058-BF2B-4D41-8FF3-F9B3CC75F6C8}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.70</cx:f>
+              <cx:f>_xlchart.v1.32</cx:f>
               <cx:v>I play longer than I meant to</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4580,7 +4580,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{E0422A26-D9DA-4370-AB44-98F821AAB3C8}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.72</cx:f>
+              <cx:f>_xlchart.v1.34</cx:f>
               <cx:v>I really get into the game</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4602,7 +4602,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{D0CCE0DE-E4ED-4C33-B35F-7825BB57E66D}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.74</cx:f>
+              <cx:f>_xlchart.v1.36</cx:f>
               <cx:v>I feel like I just can't stop playing</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4668,97 +4668,97 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.27</cx:f>
+        <cx:f>_xlchart.v1.65</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.29</cx:f>
+        <cx:f>_xlchart.v1.67</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.31</cx:f>
+        <cx:f>_xlchart.v1.69</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.33</cx:f>
+        <cx:f>_xlchart.v1.71</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="4">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.35</cx:f>
+        <cx:f>_xlchart.v1.73</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="5">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.37</cx:f>
+        <cx:f>_xlchart.v1.75</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="6">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.39</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="7">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.41</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="8">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.5</cx:f>
+        <cx:f>_xlchart.v1.43</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="9">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.7</cx:f>
+        <cx:f>_xlchart.v1.45</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="10">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.9</cx:f>
+        <cx:f>_xlchart.v1.47</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="11">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.11</cx:f>
+        <cx:f>_xlchart.v1.49</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="12">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.13</cx:f>
+        <cx:f>_xlchart.v1.51</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="13">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.15</cx:f>
+        <cx:f>_xlchart.v1.53</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="14">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.17</cx:f>
+        <cx:f>_xlchart.v1.55</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="15">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.19</cx:f>
+        <cx:f>_xlchart.v1.57</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="16">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.21</cx:f>
+        <cx:f>_xlchart.v1.59</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="17">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.23</cx:f>
+        <cx:f>_xlchart.v1.61</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="18">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.25</cx:f>
+        <cx:f>_xlchart.v1.63</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -4768,7 +4768,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{6B2C322B-B993-4F8E-AD6D-D6C2B7F63CF8}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.26</cx:f>
+              <cx:f>_xlchart.v1.64</cx:f>
               <cx:v>I lose track of time_1</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4792,7 +4792,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{E02B80E8-2FB2-4DDC-AD8F-7C1781B5351D}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.28</cx:f>
+              <cx:f>_xlchart.v1.66</cx:f>
               <cx:v>I was interested in the game's story_2</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4816,7 +4816,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{5325B789-9EA1-459B-8B3A-2BA177FA7452}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.30</cx:f>
+              <cx:f>_xlchart.v1.68</cx:f>
               <cx:v>I feel different _3</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4840,7 +4840,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{93E216F0-D381-4781-9469-3F638844AB76}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.32</cx:f>
+              <cx:f>_xlchart.v1.70</cx:f>
               <cx:v>I felt that I could explore things_19</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4864,7 +4864,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{20D76B0E-414F-4FB1-89D3-2C12891AC821}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.34</cx:f>
+              <cx:f>_xlchart.v1.72</cx:f>
               <cx:v>The game feels real_4</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4888,7 +4888,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{0613C36A-79A9-425B-A85A-BCCC0AAEAAAD}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.36</cx:f>
+              <cx:f>_xlchart.v1.74</cx:f>
               <cx:v>I was fully occupied with the game_5</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4912,7 +4912,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{9BF60487-8D59-4343-B646-2B08CC91102F}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.0</cx:f>
+              <cx:f>_xlchart.v1.38</cx:f>
               <cx:v>I get wound up_6</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4936,7 +4936,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{3C11C9EF-0425-4EF0-8A74-AEFF33F41B94}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.2</cx:f>
+              <cx:f>_xlchart.v1.40</cx:f>
               <cx:v>Time seems to kind of stand still or stop_7</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4960,7 +4960,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{B63E5641-6ECE-49B4-9F68-EA30F58B69D5}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.4</cx:f>
+              <cx:f>_xlchart.v1.42</cx:f>
               <cx:v>I feel spaced out_8</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4984,7 +4984,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{54428096-C2D4-4AEF-945F-A64229B05518}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.6</cx:f>
+              <cx:f>_xlchart.v1.44</cx:f>
               <cx:v>I was deeply concentrated in the game_9</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5008,7 +5008,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{BB6AC2EE-2865-4768-AC7D-B362833BF49C}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.8</cx:f>
+              <cx:f>_xlchart.v1.46</cx:f>
               <cx:v>I got tired_10</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5032,7 +5032,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{F995007B-3A0D-4C3A-9571-70C97B54984D}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.10</cx:f>
+              <cx:f>_xlchart.v1.48</cx:f>
               <cx:v>Playing seems automatic_11</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5056,7 +5056,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{D1C795A9-A8BC-4834-A07C-A2DC95455B20}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.12</cx:f>
+              <cx:f>_xlchart.v1.50</cx:f>
               <cx:v>My thoughts go fast_12</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5080,7 +5080,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{AA2769E5-103B-4214-ACCF-F279E62AA73F}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.14</cx:f>
+              <cx:f>_xlchart.v1.52</cx:f>
               <cx:v>I enjoyed it_13</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5104,7 +5104,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{698B5BAD-519B-4E6E-9009-39D5E773E964}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.16</cx:f>
+              <cx:f>_xlchart.v1.54</cx:f>
               <cx:v>I play without thinking how to play_14</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5128,7 +5128,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{AE8BED53-DB07-4840-A396-E6DA970FBB0C}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.18</cx:f>
+              <cx:f>_xlchart.v1.56</cx:f>
               <cx:v>Playing makes me feel calm_15</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5152,7 +5152,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{F95B28B1-4041-45E4-8DF6-E9AAE288F2EE}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.20</cx:f>
+              <cx:f>_xlchart.v1.58</cx:f>
               <cx:v>I play longer than I meant to_16</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5176,7 +5176,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{D3FD1AF5-FA39-4C5C-A16C-5B0200C2A3D1}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.22</cx:f>
+              <cx:f>_xlchart.v1.60</cx:f>
               <cx:v>I really get into the game_17</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5200,7 +5200,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{10B828E5-ACEC-4185-99CE-BAF84DF0A917}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.24</cx:f>
+              <cx:f>_xlchart.v1.62</cx:f>
               <cx:v>I feel like I just can't stop playing_18</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5242,97 +5242,97 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.77</cx:f>
+        <cx:f>_xlchart.v1.115</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.79</cx:f>
+        <cx:f>_xlchart.v1.117</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.81</cx:f>
+        <cx:f>_xlchart.v1.119</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.83</cx:f>
+        <cx:f>_xlchart.v1.121</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="4">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.85</cx:f>
+        <cx:f>_xlchart.v1.123</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="5">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.87</cx:f>
+        <cx:f>_xlchart.v1.125</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="6">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.89</cx:f>
+        <cx:f>_xlchart.v1.127</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="7">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.91</cx:f>
+        <cx:f>_xlchart.v1.129</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="8">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.93</cx:f>
+        <cx:f>_xlchart.v1.131</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="9">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.95</cx:f>
+        <cx:f>_xlchart.v1.133</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="10">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.97</cx:f>
+        <cx:f>_xlchart.v1.135</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="11">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.99</cx:f>
+        <cx:f>_xlchart.v1.137</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="12">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.101</cx:f>
+        <cx:f>_xlchart.v1.139</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="13">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.103</cx:f>
+        <cx:f>_xlchart.v1.141</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="14">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.105</cx:f>
+        <cx:f>_xlchart.v1.143</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="15">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.107</cx:f>
+        <cx:f>_xlchart.v1.145</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="16">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.109</cx:f>
+        <cx:f>_xlchart.v1.147</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="17">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.111</cx:f>
+        <cx:f>_xlchart.v1.149</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="18">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.113</cx:f>
+        <cx:f>_xlchart.v1.151</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -5342,7 +5342,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{B71226A2-0FD7-4A7F-B584-69747636A850}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.76</cx:f>
+              <cx:f>_xlchart.v1.114</cx:f>
               <cx:v>I lose track of time_1</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5366,7 +5366,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{4438934A-17F4-4C46-A258-6CCA9A6AAEE2}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.78</cx:f>
+              <cx:f>_xlchart.v1.116</cx:f>
               <cx:v>I was interested in the game's story_2</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5390,7 +5390,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{1FF4E36A-E2C9-4D43-89E2-0794D3A5507C}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.80</cx:f>
+              <cx:f>_xlchart.v1.118</cx:f>
               <cx:v>I feel different _3</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5414,7 +5414,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{7E2C3773-031F-4E4A-A600-4BEEB30A2842}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.82</cx:f>
+              <cx:f>_xlchart.v1.120</cx:f>
               <cx:v>I felt that I could explore things_19</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5438,7 +5438,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{15C882DE-C1F6-4C8A-B8F5-E488E7F9B696}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.84</cx:f>
+              <cx:f>_xlchart.v1.122</cx:f>
               <cx:v>The game feels real_4</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5462,7 +5462,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{8C643387-B1F0-48D2-BFD9-029450868CBF}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.86</cx:f>
+              <cx:f>_xlchart.v1.124</cx:f>
               <cx:v>I was fully occupied with the game_5</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5486,7 +5486,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{C726DA54-373D-4575-A283-14DFA18FDF60}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.88</cx:f>
+              <cx:f>_xlchart.v1.126</cx:f>
               <cx:v>I get wound up_6</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5510,7 +5510,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{CB753087-38D1-415F-A67C-F6D1C965A876}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.90</cx:f>
+              <cx:f>_xlchart.v1.128</cx:f>
               <cx:v>Time seems to kind of stand still or stop_7</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5534,7 +5534,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{33DD0E8A-976A-43B6-B797-B7D7FB41AEB0}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.92</cx:f>
+              <cx:f>_xlchart.v1.130</cx:f>
               <cx:v>I feel spaced out_8</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5558,7 +5558,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{837617D6-F352-488B-9D42-26E1A471848F}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.94</cx:f>
+              <cx:f>_xlchart.v1.132</cx:f>
               <cx:v>I was deeply concentrated in the game_9</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5582,7 +5582,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{F004EC9D-1A45-4B71-8B2B-1B716AC335C1}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.96</cx:f>
+              <cx:f>_xlchart.v1.134</cx:f>
               <cx:v>I got tired_10</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5606,7 +5606,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{B61728EC-71A4-4AC8-8B85-0351777A9908}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.98</cx:f>
+              <cx:f>_xlchart.v1.136</cx:f>
               <cx:v>Playing seems automatic_11</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5630,7 +5630,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{DFC2FCFC-3149-467B-9B69-2B05E046EBB0}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.100</cx:f>
+              <cx:f>_xlchart.v1.138</cx:f>
               <cx:v>My thoughts go fast_12</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5654,7 +5654,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{F7F352DD-C01E-4289-84BB-B062B1347E79}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.102</cx:f>
+              <cx:f>_xlchart.v1.140</cx:f>
               <cx:v>I enjoyed it_13</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5678,7 +5678,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{562A32E3-31F3-49B1-8FE0-9E1079F9E882}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.104</cx:f>
+              <cx:f>_xlchart.v1.142</cx:f>
               <cx:v>I play without thinking how to play_14</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5702,7 +5702,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{944F3130-1904-4E51-97A2-D610FAFFEE4D}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.106</cx:f>
+              <cx:f>_xlchart.v1.144</cx:f>
               <cx:v>Playing makes me feel calm_15</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5726,7 +5726,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{6CB22AA3-AB90-40DB-884B-F6A2ADBB5A09}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.108</cx:f>
+              <cx:f>_xlchart.v1.146</cx:f>
               <cx:v>I play longer than I meant to_16</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5750,7 +5750,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{D4665FFD-BF85-4A44-B4E8-4EE594665D69}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.110</cx:f>
+              <cx:f>_xlchart.v1.148</cx:f>
               <cx:v>I really get into the game_17</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5774,7 +5774,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{881A8826-539A-4798-91B8-A059E5DF96A3}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.112</cx:f>
+              <cx:f>_xlchart.v1.150</cx:f>
               <cx:v>I feel like I just can't stop playing_18</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5816,97 +5816,97 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.141</cx:f>
+        <cx:f>_xlchart.v1.103</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.143</cx:f>
+        <cx:f>_xlchart.v1.105</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.145</cx:f>
+        <cx:f>_xlchart.v1.107</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.147</cx:f>
+        <cx:f>_xlchart.v1.109</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="4">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.149</cx:f>
+        <cx:f>_xlchart.v1.111</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="5">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.151</cx:f>
+        <cx:f>_xlchart.v1.113</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="6">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.115</cx:f>
+        <cx:f>_xlchart.v1.77</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="7">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.117</cx:f>
+        <cx:f>_xlchart.v1.79</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="8">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.119</cx:f>
+        <cx:f>_xlchart.v1.81</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="9">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.121</cx:f>
+        <cx:f>_xlchart.v1.83</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="10">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.123</cx:f>
+        <cx:f>_xlchart.v1.85</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="11">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.125</cx:f>
+        <cx:f>_xlchart.v1.87</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="12">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.127</cx:f>
+        <cx:f>_xlchart.v1.89</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="13">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.129</cx:f>
+        <cx:f>_xlchart.v1.91</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="14">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.131</cx:f>
+        <cx:f>_xlchart.v1.93</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="15">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.133</cx:f>
+        <cx:f>_xlchart.v1.95</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="16">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.135</cx:f>
+        <cx:f>_xlchart.v1.97</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="17">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.137</cx:f>
+        <cx:f>_xlchart.v1.99</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="18">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.139</cx:f>
+        <cx:f>_xlchart.v1.101</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -5916,7 +5916,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{D4FF7C23-5FDB-48C6-86D8-2976A7CA21D3}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.140</cx:f>
+              <cx:f>_xlchart.v1.102</cx:f>
               <cx:v>I lose track of time</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5940,7 +5940,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{79745BDB-A86E-497F-B533-959F50026377}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.142</cx:f>
+              <cx:f>_xlchart.v1.104</cx:f>
               <cx:v>I was interested in the game's story</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5964,7 +5964,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{912E1900-FE5B-4A19-80A4-1D1D9281AB97}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.144</cx:f>
+              <cx:f>_xlchart.v1.106</cx:f>
               <cx:v>I feel different </cx:v>
             </cx:txData>
           </cx:tx>
@@ -5988,7 +5988,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{449F0046-4F1D-4CA3-8326-D55B2A84370B}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.146</cx:f>
+              <cx:f>_xlchart.v1.108</cx:f>
               <cx:v>I felt that I could explore things</cx:v>
             </cx:txData>
           </cx:tx>
@@ -6012,7 +6012,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{E566A8AA-FE17-4837-9500-DD8746CA9F32}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.148</cx:f>
+              <cx:f>_xlchart.v1.110</cx:f>
               <cx:v>The game feels real</cx:v>
             </cx:txData>
           </cx:tx>
@@ -6036,7 +6036,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{B56FCFAF-955F-4F30-B331-9500770B017E}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.150</cx:f>
+              <cx:f>_xlchart.v1.112</cx:f>
               <cx:v>I was fully occupied with the game</cx:v>
             </cx:txData>
           </cx:tx>
@@ -6060,7 +6060,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{F93E0A56-731D-498D-80DD-0903E0B8A135}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.114</cx:f>
+              <cx:f>_xlchart.v1.76</cx:f>
               <cx:v>I get wound up</cx:v>
             </cx:txData>
           </cx:tx>
@@ -6084,7 +6084,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{13660BC4-D8ED-4338-B6FD-D87478EF1D69}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.116</cx:f>
+              <cx:f>_xlchart.v1.78</cx:f>
               <cx:v>Time seems to kind of stand still or stop</cx:v>
             </cx:txData>
           </cx:tx>
@@ -6108,7 +6108,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{02C41259-583A-4B2C-95E1-96EA73311E87}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.118</cx:f>
+              <cx:f>_xlchart.v1.80</cx:f>
               <cx:v>I feel spaced out</cx:v>
             </cx:txData>
           </cx:tx>
@@ -6132,7 +6132,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{C99AC0CE-A9D1-4E63-8E58-B77CE838ACD2}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.120</cx:f>
+              <cx:f>_xlchart.v1.82</cx:f>
               <cx:v>I was deeply concentrated in the game</cx:v>
             </cx:txData>
           </cx:tx>
@@ -6156,7 +6156,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{1B5E4F9A-140B-4980-A045-686916C697AD}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.122</cx:f>
+              <cx:f>_xlchart.v1.84</cx:f>
               <cx:v>I got tired</cx:v>
             </cx:txData>
           </cx:tx>
@@ -6180,7 +6180,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{23B502A3-565E-4E97-A7C7-30CE86C6EB71}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.124</cx:f>
+              <cx:f>_xlchart.v1.86</cx:f>
               <cx:v>Playing seems automatic</cx:v>
             </cx:txData>
           </cx:tx>
@@ -6204,7 +6204,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{19D417AC-B749-4C9B-8400-21BF41766188}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.126</cx:f>
+              <cx:f>_xlchart.v1.88</cx:f>
               <cx:v>My thoughts go fast</cx:v>
             </cx:txData>
           </cx:tx>
@@ -6228,7 +6228,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{697410DD-90B5-413E-8296-D8D0CF4C58B3}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.128</cx:f>
+              <cx:f>_xlchart.v1.90</cx:f>
               <cx:v>I enjoyed it</cx:v>
             </cx:txData>
           </cx:tx>
@@ -6252,7 +6252,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{947BDBA6-CFB0-44ED-8AC0-06ED7B3B27A5}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.130</cx:f>
+              <cx:f>_xlchart.v1.92</cx:f>
               <cx:v>I play without thinking how to play</cx:v>
             </cx:txData>
           </cx:tx>
@@ -6276,7 +6276,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{38BCB0F4-587D-4299-94C0-DAA498217636}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.132</cx:f>
+              <cx:f>_xlchart.v1.94</cx:f>
               <cx:v>Playing makes me feel calm</cx:v>
             </cx:txData>
           </cx:tx>
@@ -6300,7 +6300,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{ADE931C0-FF8B-453F-8FDA-AE989011A896}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.134</cx:f>
+              <cx:f>_xlchart.v1.96</cx:f>
               <cx:v>I play longer than I meant to</cx:v>
             </cx:txData>
           </cx:tx>
@@ -6324,7 +6324,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{24E47364-F3A4-47BD-9E14-6DF07A374A3A}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.136</cx:f>
+              <cx:f>_xlchart.v1.98</cx:f>
               <cx:v>I really get into the game</cx:v>
             </cx:txData>
           </cx:tx>
@@ -6348,7 +6348,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{DAAAB185-F770-487A-930B-ADD3CCF62110}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.138</cx:f>
+              <cx:f>_xlchart.v1.100</cx:f>
               <cx:v>I feel like I just can't stop playing</cx:v>
             </cx:txData>
           </cx:tx>
@@ -14264,8 +14264,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{25630212-324B-4845-B728-9982B6D414E0}" name="Tabela przestawna3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
-  <location ref="A16:C33" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9761F5E6-B04D-4771-999E-8C2CD50A9644}" name="Tabela przestawna4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+  <location ref="E1:G7" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="54">
     <pivotField dataField="1" showAll="0"/>
     <pivotField showAll="0">
@@ -14297,24 +14297,14 @@
         <item t="default"/>
       </items>
     </pivotField>
+    <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
-      <items count="17">
-        <item x="14"/>
-        <item x="10"/>
-        <item x="5"/>
-        <item x="8"/>
-        <item x="11"/>
-        <item x="6"/>
+      <items count="6">
+        <item x="0"/>
         <item x="1"/>
-        <item x="13"/>
-        <item x="15"/>
-        <item x="0"/>
+        <item x="3"/>
         <item x="4"/>
         <item x="2"/>
-        <item x="9"/>
-        <item x="12"/>
-        <item x="3"/>
-        <item x="7"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -14365,12 +14355,11 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
   </pivotFields>
   <rowFields count="1">
-    <field x="5"/>
+    <field x="6"/>
   </rowFields>
-  <rowItems count="17">
+  <rowItems count="6">
     <i>
       <x/>
     </i>
@@ -14385,39 +14374,6 @@
     </i>
     <i>
       <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="15"/>
     </i>
     <i t="grand">
       <x/>
@@ -15277,6 +15233,204 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{25630212-324B-4845-B728-9982B6D414E0}" name="Tabela przestawna3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+  <location ref="A16:C33" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="54">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="9">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="17">
+        <item x="14"/>
+        <item x="10"/>
+        <item x="5"/>
+        <item x="8"/>
+        <item x="11"/>
+        <item x="6"/>
+        <item x="1"/>
+        <item x="13"/>
+        <item x="15"/>
+        <item x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="9"/>
+        <item x="12"/>
+        <item x="3"/>
+        <item x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="5"/>
+  </rowFields>
+  <rowItems count="17">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Liczba z Sygnatura czasowa" fld="0" subtotal="count" baseField="3" baseItem="0"/>
+    <dataField name="Liczba z Sygnatura czasowa2" fld="0" subtotal="count" showDataAs="percentOfTotal" baseField="3" baseItem="0" numFmtId="10"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{525D8E6B-4ACF-4E1E-AFB7-1429A33723B8}" name="Tabela przestawna2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A7:C14" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="54">
@@ -15424,7 +15578,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BDC3BF1C-0AFD-43F0-8F48-66E1C8D0E42D}" name="Tabela przestawna1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A1:C5" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="54">
@@ -15563,7 +15717,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{09956D78-D7CD-4AB2-BB04-C4ABF9A75F6E}" name="Tabela przestawna5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="E9:G15" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="54">
@@ -15658,160 +15812,6 @@
   </pivotFields>
   <rowFields count="1">
     <field x="7"/>
-  </rowFields>
-  <rowItems count="6">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Liczba z Sygnatura czasowa" fld="0" subtotal="count" baseField="3" baseItem="0"/>
-    <dataField name="Liczba z Sygnatura czasowa2" fld="0" subtotal="count" showDataAs="percentOfTotal" baseField="3" baseItem="0" numFmtId="10"/>
-  </dataFields>
-  <chartFormats count="1">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9761F5E6-B04D-4771-999E-8C2CD50A9644}" name="Tabela przestawna4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
-  <location ref="E1:G7" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="54">
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="9">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="6"/>
   </rowFields>
   <rowItems count="6">
     <i>
@@ -23272,14 +23272,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56301FEA-F6F1-417A-B5B6-9A3FB80D9B06}">
   <dimension ref="A1:AM18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:A18"/>
+    <sheetView topLeftCell="AA1" workbookViewId="0">
+      <selection activeCell="AG16" sqref="AG16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.25">
@@ -25024,24 +25024,24 @@
     </row>
     <row r="16" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f>AVERAGE(A2:A15)</f>
+        <f>ROUND(AVERAGE(A2:A15),2)</f>
         <v>3</v>
       </c>
       <c r="B16">
-        <f t="shared" ref="B16:S16" si="0">AVERAGE(B2:B15)</f>
-        <v>3.1428571428571428</v>
+        <f t="shared" ref="B16:S16" si="0">ROUND(AVERAGE(B2:B15),2)</f>
+        <v>3.14</v>
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>2.5714285714285716</v>
+        <v>2.57</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>1.8571428571428572</v>
+        <v>1.86</v>
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
-        <v>2.1428571428571428</v>
+        <v>2.14</v>
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
@@ -25049,27 +25049,27 @@
       </c>
       <c r="G16">
         <f t="shared" si="0"/>
-        <v>2.4285714285714284</v>
+        <v>2.4300000000000002</v>
       </c>
       <c r="H16">
         <f t="shared" si="0"/>
-        <v>2.2142857142857144</v>
+        <v>2.21</v>
       </c>
       <c r="I16">
         <f t="shared" si="0"/>
-        <v>2.4285714285714284</v>
+        <v>2.4300000000000002</v>
       </c>
       <c r="J16">
         <f t="shared" si="0"/>
-        <v>2.9285714285714284</v>
+        <v>2.93</v>
       </c>
       <c r="K16">
         <f t="shared" si="0"/>
-        <v>3.2857142857142856</v>
+        <v>3.29</v>
       </c>
       <c r="L16">
         <f t="shared" si="0"/>
-        <v>3.2857142857142856</v>
+        <v>3.29</v>
       </c>
       <c r="M16">
         <f t="shared" si="0"/>
@@ -25077,11 +25077,11 @@
       </c>
       <c r="N16">
         <f t="shared" si="0"/>
-        <v>3.3571428571428572</v>
+        <v>3.36</v>
       </c>
       <c r="O16">
         <f t="shared" si="0"/>
-        <v>3.7142857142857144</v>
+        <v>3.71</v>
       </c>
       <c r="P16">
         <f t="shared" si="0"/>
@@ -25089,31 +25089,31 @@
       </c>
       <c r="Q16">
         <f t="shared" si="0"/>
-        <v>2.6428571428571428</v>
+        <v>2.64</v>
       </c>
       <c r="R16">
         <f t="shared" si="0"/>
-        <v>3.0714285714285716</v>
+        <v>3.07</v>
       </c>
       <c r="S16">
         <f t="shared" si="0"/>
-        <v>2.2142857142857144</v>
+        <v>2.21</v>
       </c>
       <c r="U16">
-        <f>AVERAGE(U2:U15)</f>
-        <v>2.6428571428571428</v>
+        <f>ROUND(AVERAGE(U2:U15),2)</f>
+        <v>2.64</v>
       </c>
       <c r="V16">
-        <f t="shared" ref="V16:AM16" si="1">AVERAGE(V2:V15)</f>
-        <v>3.0714285714285716</v>
+        <f t="shared" ref="V16:AM16" si="1">ROUND(AVERAGE(V2:V15),2)</f>
+        <v>3.07</v>
       </c>
       <c r="W16">
         <f t="shared" si="1"/>
-        <v>2.8571428571428572</v>
+        <v>2.86</v>
       </c>
       <c r="X16">
         <f t="shared" si="1"/>
-        <v>3.7857142857142856</v>
+        <v>3.79</v>
       </c>
       <c r="Y16">
         <f t="shared" si="1"/>
@@ -25121,19 +25121,19 @@
       </c>
       <c r="Z16">
         <f t="shared" si="1"/>
-        <v>2.9285714285714284</v>
+        <v>2.93</v>
       </c>
       <c r="AA16">
         <f t="shared" si="1"/>
-        <v>2.6428571428571428</v>
+        <v>2.64</v>
       </c>
       <c r="AB16">
         <f t="shared" si="1"/>
-        <v>2.3571428571428572</v>
+        <v>2.36</v>
       </c>
       <c r="AC16">
         <f t="shared" si="1"/>
-        <v>2.2857142857142856</v>
+        <v>2.29</v>
       </c>
       <c r="AD16">
         <f t="shared" si="1"/>
@@ -25145,35 +25145,35 @@
       </c>
       <c r="AF16">
         <f t="shared" si="1"/>
-        <v>2.2857142857142856</v>
+        <v>2.29</v>
       </c>
       <c r="AG16">
         <f t="shared" si="1"/>
-        <v>2.6428571428571428</v>
+        <v>2.64</v>
       </c>
       <c r="AH16">
         <f t="shared" si="1"/>
-        <v>3.2857142857142856</v>
+        <v>3.29</v>
       </c>
       <c r="AI16">
         <f t="shared" si="1"/>
-        <v>2.9285714285714284</v>
+        <v>2.93</v>
       </c>
       <c r="AJ16">
         <f t="shared" si="1"/>
-        <v>2.7857142857142856</v>
+        <v>2.79</v>
       </c>
       <c r="AK16">
         <f t="shared" si="1"/>
-        <v>2.7142857142857144</v>
+        <v>2.71</v>
       </c>
       <c r="AL16">
         <f t="shared" si="1"/>
-        <v>3.0714285714285716</v>
+        <v>3.07</v>
       </c>
       <c r="AM16">
         <f t="shared" si="1"/>
-        <v>2.1428571428571428</v>
+        <v>2.14</v>
       </c>
     </row>
     <row r="17" spans="1:39" x14ac:dyDescent="0.25">
@@ -25332,156 +25332,156 @@
     </row>
     <row r="18" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f>_xlfn.STDEV.S(A2:A15)</f>
-        <v>1.2403473458920846</v>
+        <f>ROUND(_xlfn.STDEV.S(A2:A15),2)</f>
+        <v>1.24</v>
       </c>
       <c r="B18">
-        <f t="shared" ref="B18:S18" si="4">_xlfn.STDEV.S(B2:B15)</f>
-        <v>1.2924123453177283</v>
+        <f t="shared" ref="B18:S18" si="4">ROUND(_xlfn.STDEV.S(B2:B15),2)</f>
+        <v>1.29</v>
       </c>
       <c r="C18">
         <f t="shared" si="4"/>
-        <v>1.4525460784051258</v>
+        <v>1.45</v>
       </c>
       <c r="D18">
         <f t="shared" si="4"/>
-        <v>1.1673205911990769</v>
+        <v>1.17</v>
       </c>
       <c r="E18">
         <f t="shared" si="4"/>
-        <v>1.2314558524297636</v>
+        <v>1.23</v>
       </c>
       <c r="F18">
         <f t="shared" si="4"/>
-        <v>1.5191090506254998</v>
+        <v>1.52</v>
       </c>
       <c r="G18">
         <f t="shared" si="4"/>
-        <v>1.2838814775327387</v>
+        <v>1.28</v>
       </c>
       <c r="H18">
         <f t="shared" si="4"/>
-        <v>1.3114039117603014</v>
+        <v>1.31</v>
       </c>
       <c r="I18">
         <f t="shared" si="4"/>
-        <v>1.3424596091494905</v>
+        <v>1.34</v>
       </c>
       <c r="J18">
         <f t="shared" si="4"/>
-        <v>1.3847680013570567</v>
+        <v>1.38</v>
       </c>
       <c r="K18">
         <f t="shared" si="4"/>
-        <v>1.5406577730392867</v>
+        <v>1.54</v>
       </c>
       <c r="L18">
         <f t="shared" si="4"/>
-        <v>1.266647387553302</v>
+        <v>1.27</v>
       </c>
       <c r="M18">
         <f t="shared" si="4"/>
-        <v>1.3008872711759818</v>
+        <v>1.3</v>
       </c>
       <c r="N18">
         <f t="shared" si="4"/>
-        <v>1.3363062095621221</v>
+        <v>1.34</v>
       </c>
       <c r="O18">
         <f t="shared" si="4"/>
-        <v>1.4373357526806554</v>
+        <v>1.44</v>
       </c>
       <c r="P18">
         <f t="shared" si="4"/>
-        <v>1.2403473458920846</v>
+        <v>1.24</v>
       </c>
       <c r="Q18">
         <f t="shared" si="4"/>
-        <v>1.4990839693802167</v>
+        <v>1.5</v>
       </c>
       <c r="R18">
         <f t="shared" si="4"/>
-        <v>1.3280573269766116</v>
+        <v>1.33</v>
       </c>
       <c r="S18">
         <f t="shared" si="4"/>
-        <v>1.4769288003552106</v>
+        <v>1.48</v>
       </c>
       <c r="U18">
-        <f>_xlfn.STDEV.S(U2:U15)</f>
-        <v>1.3363062095621216</v>
+        <f>ROUND(_xlfn.STDEV.S(U2:U15),2)</f>
+        <v>1.34</v>
       </c>
       <c r="V18">
-        <f t="shared" ref="V18:AM18" si="5">_xlfn.STDEV.S(V2:V15)</f>
-        <v>1.4392458342578485</v>
+        <f t="shared" ref="V18:AM18" si="5">ROUND(_xlfn.STDEV.S(V2:V15),2)</f>
+        <v>1.44</v>
       </c>
       <c r="W18">
         <f t="shared" si="5"/>
-        <v>1.4600918230947433</v>
+        <v>1.46</v>
       </c>
       <c r="X18">
         <f t="shared" si="5"/>
-        <v>1.3688047244316386</v>
+        <v>1.37</v>
       </c>
       <c r="Y18">
         <f t="shared" si="5"/>
-        <v>1.4142135623730951</v>
+        <v>1.41</v>
       </c>
       <c r="Z18">
         <f t="shared" si="5"/>
-        <v>1.4917354742965407</v>
+        <v>1.49</v>
       </c>
       <c r="AA18">
         <f t="shared" si="5"/>
-        <v>1.5984195491000022</v>
+        <v>1.6</v>
       </c>
       <c r="AB18">
         <f t="shared" si="5"/>
-        <v>1.4468609447374661</v>
+        <v>1.45</v>
       </c>
       <c r="AC18">
         <f t="shared" si="5"/>
-        <v>1.3827826698682308</v>
+        <v>1.38</v>
       </c>
       <c r="AD18">
         <f t="shared" si="5"/>
-        <v>1.6172150801252798</v>
+        <v>1.62</v>
       </c>
       <c r="AE18">
         <f t="shared" si="5"/>
-        <v>1.2247448713915889</v>
+        <v>1.22</v>
       </c>
       <c r="AF18">
         <f t="shared" si="5"/>
-        <v>1.1387288073563859</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="AG18">
         <f t="shared" si="5"/>
-        <v>1.3363062095621216</v>
+        <v>1.34</v>
       </c>
       <c r="AH18">
         <f t="shared" si="5"/>
-        <v>1.4373357526806554</v>
+        <v>1.44</v>
       </c>
       <c r="AI18">
         <f t="shared" si="5"/>
-        <v>1.4917354742965407</v>
+        <v>1.49</v>
       </c>
       <c r="AJ18">
         <f t="shared" si="5"/>
-        <v>1.2513728724621076</v>
+        <v>1.25</v>
       </c>
       <c r="AK18">
         <f t="shared" si="5"/>
-        <v>1.489892687336984</v>
+        <v>1.49</v>
       </c>
       <c r="AL18">
         <f t="shared" si="5"/>
-        <v>1.3847680013570565</v>
+        <v>1.38</v>
       </c>
       <c r="AM18">
         <f t="shared" si="5"/>
-        <v>1.4600918230947433</v>
+        <v>1.46</v>
       </c>
     </row>
   </sheetData>
@@ -25494,8 +25494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96C7CF50-2FBD-4111-B95C-9FFDFC7A48D3}">
   <dimension ref="A1:AM24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="AN21" sqref="AN21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T22" sqref="T22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27938,11 +27938,11 @@
     </row>
     <row r="22" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f>AVERAGE(A2:A21)</f>
+        <f>ROUND(AVERAGE(A2:A21),2)</f>
         <v>3.7</v>
       </c>
       <c r="B22">
-        <f t="shared" ref="B22:S22" si="0">AVERAGE(B2:B21)</f>
+        <f t="shared" ref="B22:S22" si="0">ROUND(AVERAGE(B2:B21),2)</f>
         <v>3.8</v>
       </c>
       <c r="C22">
@@ -28014,11 +28014,11 @@
         <v>3.15</v>
       </c>
       <c r="U22">
-        <f>AVERAGE(U2:U21)</f>
+        <f>ROUND(AVERAGE(U2:U21),2)</f>
         <v>3.1</v>
       </c>
       <c r="V22">
-        <f t="shared" ref="V22:AM22" si="1">AVERAGE(V2:V21)</f>
+        <f t="shared" ref="V22:AM22" si="1">ROUND(AVERAGE(V2:V21),2)</f>
         <v>3.5</v>
       </c>
       <c r="W22">
@@ -28246,156 +28246,156 @@
     </row>
     <row r="24" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f>_xlfn.STDEV.S(A2:A21)</f>
-        <v>1.2607433062326865</v>
+        <f>ROUND(_xlfn.STDEV.S(A2:A21),2)</f>
+        <v>1.26</v>
       </c>
       <c r="B24">
-        <f t="shared" ref="B24:S24" si="4">_xlfn.STDEV.S(B2:B21)</f>
-        <v>1.1516578439248715</v>
+        <f t="shared" ref="B24:S24" si="4">ROUND(_xlfn.STDEV.S(B2:B21),2)</f>
+        <v>1.1499999999999999</v>
       </c>
       <c r="C24">
         <f t="shared" si="4"/>
-        <v>1.4964871146156009</v>
+        <v>1.5</v>
       </c>
       <c r="D24">
         <f t="shared" si="4"/>
-        <v>1.5183093090324964</v>
+        <v>1.52</v>
       </c>
       <c r="E24">
         <f t="shared" si="4"/>
-        <v>1.3337718577107005</v>
+        <v>1.33</v>
       </c>
       <c r="F24">
         <f t="shared" si="4"/>
-        <v>1.3869694338832115</v>
+        <v>1.39</v>
       </c>
       <c r="G24">
         <f t="shared" si="4"/>
-        <v>1.5517392618742702</v>
+        <v>1.55</v>
       </c>
       <c r="H24">
         <f t="shared" si="4"/>
-        <v>1.4363696929192156</v>
+        <v>1.44</v>
       </c>
       <c r="I24">
         <f t="shared" si="4"/>
-        <v>1.2814465510343747</v>
+        <v>1.28</v>
       </c>
       <c r="J24">
         <f t="shared" si="4"/>
-        <v>1.2732056517228267</v>
+        <v>1.27</v>
       </c>
       <c r="K24">
         <f t="shared" si="4"/>
-        <v>1.2814465510343747</v>
+        <v>1.28</v>
       </c>
       <c r="L24">
         <f t="shared" si="4"/>
-        <v>1.4363696929192156</v>
+        <v>1.44</v>
       </c>
       <c r="M24">
         <f t="shared" si="4"/>
-        <v>1.4327007988227578</v>
+        <v>1.43</v>
       </c>
       <c r="N24">
         <f t="shared" si="4"/>
-        <v>0.88704120832301658</v>
+        <v>0.89</v>
       </c>
       <c r="O24">
         <f t="shared" si="4"/>
-        <v>1.2732056517228267</v>
+        <v>1.27</v>
       </c>
       <c r="P24">
         <f t="shared" si="4"/>
-        <v>0.95145318218750852</v>
+        <v>0.95</v>
       </c>
       <c r="Q24">
         <f t="shared" si="4"/>
-        <v>1.2513150976809202</v>
+        <v>1.25</v>
       </c>
       <c r="R24">
         <f t="shared" si="4"/>
-        <v>1.2680278927697552</v>
+        <v>1.27</v>
       </c>
       <c r="S24">
         <f t="shared" si="4"/>
-        <v>1.4964871146156009</v>
+        <v>1.5</v>
       </c>
       <c r="U24">
-        <f>_xlfn.STDEV.S(U2:U21)</f>
-        <v>1.4473205733717958</v>
+        <f>ROUND(_xlfn.STDEV.S(U2:U21),2)</f>
+        <v>1.45</v>
       </c>
       <c r="V24">
-        <f t="shared" ref="V24:AM24" si="5">_xlfn.STDEV.S(V2:V21)</f>
-        <v>1.3178930553209385</v>
+        <f t="shared" ref="V24:AM24" si="5">ROUND(_xlfn.STDEV.S(V2:V21),2)</f>
+        <v>1.32</v>
       </c>
       <c r="W24">
         <f t="shared" si="5"/>
-        <v>1.7614288458371994</v>
+        <v>1.76</v>
       </c>
       <c r="X24">
         <f t="shared" si="5"/>
-        <v>1.4653901941300931</v>
+        <v>1.47</v>
       </c>
       <c r="Y24">
         <f t="shared" si="5"/>
-        <v>1.4095538674570611</v>
+        <v>1.41</v>
       </c>
       <c r="Z24">
         <f t="shared" si="5"/>
-        <v>1.4689774459950382</v>
+        <v>1.47</v>
       </c>
       <c r="AA24">
         <f t="shared" si="5"/>
-        <v>1.5252264715358452</v>
+        <v>1.53</v>
       </c>
       <c r="AB24">
         <f t="shared" si="5"/>
-        <v>1.6189665319514632</v>
+        <v>1.62</v>
       </c>
       <c r="AC24">
         <f t="shared" si="5"/>
-        <v>1.5525869752736798</v>
+        <v>1.55</v>
       </c>
       <c r="AD24">
         <f t="shared" si="5"/>
-        <v>1.3572417850765923</v>
+        <v>1.36</v>
       </c>
       <c r="AE24">
         <f t="shared" si="5"/>
-        <v>1.5008769366431645</v>
+        <v>1.5</v>
       </c>
       <c r="AF24">
         <f t="shared" si="5"/>
-        <v>0.98808693416808457</v>
+        <v>0.99</v>
       </c>
       <c r="AG24">
         <f t="shared" si="5"/>
-        <v>1.4244112357114618</v>
+        <v>1.42</v>
       </c>
       <c r="AH24">
         <f t="shared" si="5"/>
-        <v>1.1821033884786187</v>
+        <v>1.18</v>
       </c>
       <c r="AI24">
         <f t="shared" si="5"/>
-        <v>0.81272770088724933</v>
+        <v>0.81</v>
       </c>
       <c r="AJ24">
         <f t="shared" si="5"/>
-        <v>1.1742858972247994</v>
+        <v>1.17</v>
       </c>
       <c r="AK24">
         <f t="shared" si="5"/>
-        <v>1.6375527311718607</v>
+        <v>1.64</v>
       </c>
       <c r="AL24">
         <f t="shared" si="5"/>
-        <v>1.4290224851827544</v>
+        <v>1.43</v>
       </c>
       <c r="AM24">
         <f t="shared" si="5"/>
-        <v>1.5894388284780525</v>
+        <v>1.59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>